<commit_message>
GraphicEngine adding operations 3
</commit_message>
<xml_diff>
--- a/TornadoEngine/Doc/Plans/План.xlsx
+++ b/TornadoEngine/Doc/Plans/План.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11955"/>
@@ -12,26 +12,14 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
-  <si>
-    <t>Physic Engine</t>
-  </si>
-  <si>
-    <t>Game Realize (компоновка частей)</t>
-  </si>
-  <si>
-    <t>SoundEngine</t>
-  </si>
-  <si>
-    <t>Effects BigJack</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Срок</t>
   </si>
@@ -39,103 +27,31 @@
     <t>1 месяц</t>
   </si>
   <si>
-    <t>3-4 месяца</t>
-  </si>
-  <si>
-    <t>Оптимизация BigJack</t>
-  </si>
-  <si>
     <t>1-2 месяца</t>
   </si>
   <si>
-    <t>Далее идут необязательные реализации</t>
-  </si>
-  <si>
-    <t>Финальная реализация</t>
-  </si>
-  <si>
     <t>Примечания</t>
   </si>
   <si>
-    <t>Модуль</t>
-  </si>
-  <si>
-    <t>доработка компонента модуля</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Рекомендации</t>
   </si>
   <si>
     <t>Статус</t>
   </si>
   <si>
-    <t>StarTeam</t>
-  </si>
-  <si>
-    <t>1 неделя</t>
-  </si>
-  <si>
-    <t>На данном этапе лучше выпускать TornadoEngine по закрытой лицензии. Но исходники игры можно оставить под GPL (идея в том, что обзором игры можно привлечь внимание к коммерциализации или хорошему аппетиту к Tornado)</t>
-  </si>
-  <si>
-    <t>БД MySQL connector C++</t>
-  </si>
-  <si>
-    <t>2 месяца</t>
-  </si>
-  <si>
-    <t>Сервер, общая для всех игр организация, имиджы для Клиентов, комнаты и т.д.</t>
-  </si>
-  <si>
-    <t>проектирование и реализация</t>
-  </si>
-  <si>
-    <t>2 недели</t>
-  </si>
-  <si>
-    <t>в ожидании</t>
-  </si>
-  <si>
-    <t>реализация игры Tanks Demo на Клиенте и Сервере</t>
-  </si>
-  <si>
-    <t>псевдо физика и задел на будущее - требования к интерфейсу Физического движка</t>
-  </si>
-  <si>
-    <t>псевдофизика нужна для возможности реализации игры на сервере</t>
-  </si>
-  <si>
-    <t>Пост-эффекты и доведение до ума Клиента Tanks</t>
-  </si>
-  <si>
-    <t>2-4 недели</t>
-  </si>
-  <si>
     <t>Дата начала  разработки</t>
   </si>
   <si>
-    <t>начало работ</t>
-  </si>
-  <si>
-    <t>внутренний протокол обмена пакетами (игровой протокол)</t>
-  </si>
-  <si>
-    <t>Сама схема в теории готова (см. папку trash)</t>
-  </si>
-  <si>
-    <t>Класс, который обменивается сам с собой пакетами (классическая реализация, с целью инкапсуляции подробностей)</t>
-  </si>
-  <si>
-    <t>Важный этап, на нем задаются основы работы с физикой, интерфейс фасада, конвейер событий и рабочий объект среды - IBasePhysicObject</t>
-  </si>
-  <si>
-    <t>В основном это касается графики</t>
-  </si>
-  <si>
-    <t>Контур обводки(цель и т.д.), возможно оптимизация графического конвейера</t>
+    <t>Создание интерефейса GraphicEngine. Реализация на OGRE + MyGUI</t>
+  </si>
+  <si>
+    <t>1 марта 2015</t>
+  </si>
+  <si>
+    <t>Создание интерефейса PhysicEngine. Реализация на BulletEngine</t>
+  </si>
+  <si>
+    <t>1 апреля 2015</t>
   </si>
 </sst>
 </file>
@@ -180,15 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -491,217 +401,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="67.5" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3">
-        <v>41821</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
+    <row r="2" spans="1:6" ht="63.75" customHeight="1"/>
+    <row r="3" spans="1:6" ht="58.5" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="58.5" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3">
-        <v>41835</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
+    <row r="4" spans="1:6" ht="56.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75">
-      <c r="A4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3">
-        <v>41883</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="37.5">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3">
-        <v>41927</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="3">
-        <v>41958</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="37.5">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="131.25">
-      <c r="A10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="56.25">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="37.5">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="37.5">
-      <c r="A16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
+    <row r="20" ht="56.25"/>
   </sheetData>
   <pageMargins left="0.66" right="0.35433070866141736" top="0.74803149606299213" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Multi-threaded kernel of the game engine.
Developer library but does not compile :(
</commit_message>
<xml_diff>
--- a/TornadoEngine/Doc/Plans/План.xlsx
+++ b/TornadoEngine/Doc/Plans/План.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Срок</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>1 апреля 2015</t>
+  </si>
+  <si>
+    <t>В ожидании</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -435,33 +438,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63.75" customHeight="1"/>
-    <row r="3" spans="1:6" ht="58.5" customHeight="1">
+    <row r="2" spans="1:6" ht="58.5" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="56.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.1</v>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" ht="56.25"/>
   </sheetData>
   <pageMargins left="0.66" right="0.35433070866141736" top="0.74803149606299213" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>